<commit_message>
feat: test on LAN done. JD crawler expired QAQ try to fetch data from other platform
</commit_message>
<xml_diff>
--- a/crawler/good_info2.xlsx
+++ b/crawler/good_info2.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1463,6 +1463,1286 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>100111772363</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Apple/苹果【教育优惠】iPhone 13 (A2634)512GB 绿色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100111772363.html</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>6849.00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/42821/26/21396/27590/66a0df75Ff3b3bb67/e153dcc8b452c612.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>100026667880</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 128GB 午夜色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100026667880.html</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>3516.00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/225792/12/33045/27903/675b9cf5Ff3a279ab/5a62823c89ae97fe.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>100026667856</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 512GB 午夜色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100026667856.html</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>6199.00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/224468/22/39144/21706/676142ffF29393e3b/2e464feeca71e97c.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>100129853278</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Apple/苹果【12期免息】 iPhone 13 (A2634) 256GB 星光色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100129853278.html</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>5199.00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>http://img14.360buyimg.com/n1/jfs/t1/96927/39/42132/25048/66c48fd5Fd05c0ddf/4f0e769dbbc20187.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>100110442683</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Apple/苹果【24期免息】iPhone 13 (A2634) 512GB 蓝色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100110442683.html</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>7499.00</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/188196/22/44390/36906/66992c59F0b9d05c5/919fcf6e5340c05f.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>100131971674</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Apple/苹果【教育优惠】iPhone 13 (A2634)128GB 绿色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100131971674.html</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>3969.00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/80036/13/25923/27711/66a0def0F797e7ba6/3aa0c2d139660ecd.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>100019718251</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634)512GB 绿色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100019718251.html</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>5699.00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/247060/38/28908/28096/675ad534Fcf8f323b/7692a9da0e93285f.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>100129853300</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Apple/苹果【24期免息】 iPhone 13 (A2634) 512GB 粉色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100129853300.html</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>7499.00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/246067/11/15499/34840/66992c5cF80276bb1/8edb87c84010845e.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>100014352543</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 256GB 星光色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100014352543.html</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>5199.00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/240636/9/21450/23150/675ad532F49e196f0/804dedfd51feecd8.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>100014352549</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 512GB 粉色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100014352549.html</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>6199.00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/226235/13/31824/27865/675ad533Feda6f0d1/7c65228ab9e2aac4.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>100129853306</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Apple/苹果【6期免息】 iPhone 13 (A2634) 512GB 星光色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100129853306.html</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>6999.00</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/224968/28/20322/25333/66c48d45Ff823f28d/569d1973b3431e2f.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>100026667922</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 512GB 星光色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100026667922.html</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>6199.00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/236857/9/33011/27375/675ad53bF0c97e7e5/3aa12ec898755317.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>100026667908</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 512GB 红色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100026667908.html</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>5699.00</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/237481/1/27615/33312/675ad539Fe18f0bcd/6e4f18dcfbf06681.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>100034710036</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634)128GB 绿色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100034710036.html</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>3849.00</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/228013/15/30058/30225/675b9cf8Fbad3c1ce/508f049d1f99214d.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>100026667896</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 128GB 红色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100026667896.html</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>3899.00</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/201971/19/45933/32850/675b9cf6F72bb0e85/93eb82963deef704.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>100129853284</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Apple/苹果【6期免息】 iPhone 13 (A2634) 512GB 午夜色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100129853284.html</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>6999.00</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/229257/8/22104/25042/669f4294Ffb2271bb/c085dd63508d7b0b.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>100110442669</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Apple/苹果【24期免息】iPhone 13 (A2634)512GB 绿色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100110442669.html</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>7499.00</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/226585/12/22703/35323/66992c58Ff4d472cd/92c2ad349986056b.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>100111772385</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Apple/苹果【教育优惠】iPhone 13 (A2634) 512GB 粉色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100111772385.html</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>6849.00</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/235279/24/22591/27432/66a0dfbfF814300c4/6d24057efa54f91b.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>100111772355</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Apple/苹果【教育优惠】iPhone 13 (A2634) 128GB 蓝色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100111772355.html</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>3969.00</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/225281/16/24466/29739/66a0debeFaf8a9afa/fff0ad65c5634756.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>100066896526</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 (A3092) 512GB 黑色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100066896526.html</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>7899.00</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/239544/40/28830/34870/675b9d28F0f0aa8fe/c8119610e363e3c2.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>100054515243</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 14 (A2884) 512GB 黄色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100054515243.html</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>7199.00</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/184380/17/49330/39212/675b9852F4d5c5222/cb2b1a0847205343.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>100129853316</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Apple/苹果【6期免息】 iPhone 13 (A2634) 128GB 午夜色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100129853316.html</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>3999.00</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>http://img14.360buyimg.com/n1/jfs/t1/249880/5/17341/24139/66c48e8eF4c457fa3/80b5761ff937bc9f.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>100066896370</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 (A3092) 256GB 蓝色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100066896370.html</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>6249.00</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/230314/18/31781/36838/675b9d20F843fd148/77b0199fa5435eef.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>100068388597</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 1TB 蓝色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100068388597.html</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>1.06万</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/236080/21/28272/51697/675b9d1bF35597d24/cca4eaf74760e03c.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>100068388589</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 512GB 蓝色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100068388589.html</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>9099.00</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/226801/18/26406/51697/675bfb59F18a654a2/7ac3a1cddcb7e0a9.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>100110360821</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Apple/苹果【12期免息】 iPhone 13 (A2634) 256GB 粉色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100110360821.html</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>5199.00</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/87903/28/49820/25808/66c48fd9F4880200b/c22141ea3e7c1874.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>100068388451</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 256GB 原色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100068388451.html</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>8299.00</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/236756/33/28459/54934/675b98aeF53a43d61/16902e273a3a702d.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>100131971654</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Apple/苹果【教育优惠】iPhone 13 (A2634) 512GB 蓝色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100131971654.html</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>6849.00</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/82932/18/27068/29617/66a0dfadFd8fe9e60/7e5e137887ebcf45.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>100068388605</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 512GB 原色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100068388605.html</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>9399.00</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/234702/7/32457/52739/675bfb5aFfc93ab5d/d794e51a71f9a75c.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>100068388577</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 256GB 黑色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100068388577.html</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>8249.00</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/235008/25/34908/49396/675b98b0F79f3184d/3f019f82e0908a93.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>100066896356</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 (A3092) 128GB 黑色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100066896356.html</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>4999.00</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/241149/15/29166/34760/675b9d1eF4ba0a062/f802432984d292e3.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>100068388535</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 (A3092) 256GB 粉色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100068388535.html</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>6249.00</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/231513/20/34857/37001/675b9d2bF33cc3511/c5ea93e208057018.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>100066896468</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 256GB 蓝色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100066896468.html</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>8199.00</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/239425/34/27996/53892/675b9858F1582fb10/c7f6d825e5c7c4d2.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>100038005167</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 14 (A2884) 512GB 红色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100038005167.html</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>7699.00</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/238973/29/27084/42094/675b9850F986cdc8d/80d6bac64b973aeb.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>100014352525</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 128GB 蓝色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100014352525.html</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>3998.00</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/239065/30/28801/31798/675b9cf7F9f6a24b6/9f1b8bdaf48030b8.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>100067305218</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro (A3104) 512GB 蓝色钛金属 支持移动联通电信5G 双卡双待手机【快充套装】</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100067305218.html</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>9788.90</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/172522/31/40211/46154/6500da32F3d3b7cc2/cc79eb27341dd1c0.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>100066896544</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro (A3104) 1TB 白色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100066896544.html</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>9799.00</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/238968/1/28904/54806/675bfb59Fe838e691/860fa9b695379f2f.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>100066896420</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro (A3104) 256GB 蓝色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100066896420.html</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>8099.00</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/241897/2/29416/53749/675b9857Ffa06ccd3/e0148809ede317c2.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>100067304448</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 512GB 原色钛金属 支持移动联通电信5G 双卡双待手机【快充套装】</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100067304448.html</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>9188.90</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>https://img14.360buyimg.com/pop/jfs/t1/107784/5/58940/41831/6731afceF6462c0ef/4b6695694b98cb92.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>100102229845</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Apple/苹果【24期免息】iPhone 13 (A2634) 256GB 红色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100102229845.html</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>5399.00</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/248501/26/10310/28564/66583a09Fc1d7bf2d/039b4af74d9bc2c3.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update: update amazon & JD & GW cookies
</commit_message>
<xml_diff>
--- a/crawler/good_info2.xlsx
+++ b/crawler/good_info2.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2743,6 +2743,1286 @@
         </is>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>100111772363</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Apple/苹果【教育优惠】iPhone 13 (A2634)512GB 绿色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100111772363.html</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>6849.00</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/42821/26/21396/27590/66a0df75Ff3b3bb67/e153dcc8b452c612.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>100026667880</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 128GB 午夜色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100026667880.html</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>3516.00</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/225792/12/33045/27903/675b9cf5Ff3a279ab/5a62823c89ae97fe.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>100026667856</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 512GB 午夜色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100026667856.html</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>6199.00</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/224468/22/39144/21706/676142ffF29393e3b/2e464feeca71e97c.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>100129853278</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Apple/苹果【12期免息】 iPhone 13 (A2634) 256GB 星光色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100129853278.html</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>5199.00</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>http://img14.360buyimg.com/n1/jfs/t1/96927/39/42132/25048/66c48fd5Fd05c0ddf/4f0e769dbbc20187.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>100110442683</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Apple/苹果【24期免息】iPhone 13 (A2634) 512GB 蓝色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100110442683.html</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>7499.00</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/188196/22/44390/36906/66992c59F0b9d05c5/919fcf6e5340c05f.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>100131971674</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Apple/苹果【教育优惠】iPhone 13 (A2634)128GB 绿色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100131971674.html</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>3969.00</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/80036/13/25923/27711/66a0def0F797e7ba6/3aa0c2d139660ecd.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>100019718251</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634)512GB 绿色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100019718251.html</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>5699.00</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/234463/4/34265/24028/676142feFd810408d/6abeb5bcedd2f7bc.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>100129853300</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Apple/苹果【24期免息】 iPhone 13 (A2634) 512GB 粉色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100129853300.html</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>7499.00</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/246067/11/15499/34840/66992c5cF80276bb1/8edb87c84010845e.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>100014352543</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 256GB 星光色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100014352543.html</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>5199.00</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/240636/9/21450/23150/675ad532F49e196f0/804dedfd51feecd8.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>100014352549</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 512GB 粉色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100014352549.html</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>6299.00</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/226235/13/31824/27865/675ad533Feda6f0d1/7c65228ab9e2aac4.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>100129853306</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Apple/苹果【6期免息】 iPhone 13 (A2634) 512GB 星光色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100129853306.html</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>6999.00</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/224968/28/20322/25333/66c48d45Ff823f28d/569d1973b3431e2f.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>100026667922</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 512GB 星光色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100026667922.html</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>6199.00</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/230238/17/36997/23150/67614302F5078818d/9e3db2ea88982aed.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>100026667908</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 512GB 红色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100026667908.html</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>5699.00</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/241796/1/27703/26653/67614301F26d35425/d7aba6fe3321db8c.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>100034710036</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634)128GB 绿色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100034710036.html</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>3849.00</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/228013/15/30058/30225/675b9cf8Fbad3c1ce/508f049d1f99214d.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>100026667896</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 128GB 红色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100026667896.html</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>3899.00</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/201971/19/45933/32850/675b9cf6F72bb0e85/93eb82963deef704.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>100129853284</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Apple/苹果【6期免息】 iPhone 13 (A2634) 512GB 午夜色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100129853284.html</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>6999.00</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/229257/8/22104/25042/669f4294Ffb2271bb/c085dd63508d7b0b.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>100110442669</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Apple/苹果【24期免息】iPhone 13 (A2634)512GB 绿色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100110442669.html</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>7499.00</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/226585/12/22703/35323/66992c58Ff4d472cd/92c2ad349986056b.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>100111772385</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Apple/苹果【教育优惠】iPhone 13 (A2634) 512GB 粉色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100111772385.html</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>6849.00</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/235279/24/22591/27432/66a0dfbfF814300c4/6d24057efa54f91b.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>100111772355</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Apple/苹果【教育优惠】iPhone 13 (A2634) 128GB 蓝色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100111772355.html</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>3969.00</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/225281/16/24466/29739/66a0debeFaf8a9afa/fff0ad65c5634756.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>100066896526</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 (A3092) 512GB 黑色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100066896526.html</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>7899.00</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/239544/40/28830/34870/675b9d28F0f0aa8fe/c8119610e363e3c2.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>100054515243</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 14 (A2884) 512GB 黄色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100054515243.html</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>7199.00</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/184380/17/49330/39212/675b9852F4d5c5222/cb2b1a0847205343.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>100026667872</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 256GB 粉色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100026667872.html</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>5199.00</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/224322/27/24546/23766/675ad536F7f13823c/d83df466f3decfbf.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>100129853316</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Apple/苹果【6期免息】 iPhone 13 (A2634) 128GB 午夜色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100129853316.html</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>3999.00</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>http://img14.360buyimg.com/n1/jfs/t1/249880/5/17341/24139/66c48e8eF4c457fa3/80b5761ff937bc9f.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>100068388597</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 1TB 蓝色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100068388597.html</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>1.06万</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/236080/21/28272/51697/675b9d1bF35597d24/cca4eaf74760e03c.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>100068388589</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 512GB 蓝色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100068388589.html</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>9399.00</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/226801/18/26406/51697/675bfb59F18a654a2/7ac3a1cddcb7e0a9.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>100110360821</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Apple/苹果【12期免息】 iPhone 13 (A2634) 256GB 粉色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100110360821.html</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>5199.00</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/87903/28/49820/25808/66c48fd9F4880200b/c22141ea3e7c1874.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>100068388451</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 256GB 原色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100068388451.html</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>8399.00</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/236756/33/28459/54934/675b98aeF53a43d61/16902e273a3a702d.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>100131971654</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Apple/苹果【教育优惠】iPhone 13 (A2634) 512GB 蓝色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100131971654.html</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>6849.00</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/82932/18/27068/29617/66a0dfadFd8fe9e60/7e5e137887ebcf45.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>100068388605</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 512GB 原色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100068388605.html</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>9399.00</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/234702/7/32457/52739/675bfb5aFfc93ab5d/d794e51a71f9a75c.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>100068388577</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 256GB 黑色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100068388577.html</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>8249.00</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/235008/25/34908/49396/675b98b0F79f3184d/3f019f82e0908a93.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>100066896356</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 (A3092) 128GB 黑色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100066896356.html</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>4999.00</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/241149/15/29166/34760/675b9d1eF4ba0a062/f802432984d292e3.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>100068388535</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 (A3092) 256GB 粉色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100068388535.html</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>6249.00</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/231513/20/34857/37001/675b9d2bF33cc3511/c5ea93e208057018.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>100066896468</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 256GB 蓝色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100066896468.html</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>8249.00</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/239425/34/27996/53892/675b9858F1582fb10/c7f6d825e5c7c4d2.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>100038005167</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 14 (A2884) 512GB 红色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100038005167.html</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>7699.00</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/238973/29/27084/42094/675b9850F986cdc8d/80d6bac64b973aeb.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>100067305218</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro (A3104) 512GB 蓝色钛金属 支持移动联通电信5G 双卡双待手机【快充套装】</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100067305218.html</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>9888.90</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/172522/31/40211/46154/6500da32F3d3b7cc2/cc79eb27341dd1c0.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>100066896544</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro (A3104) 1TB 白色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100066896544.html</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>9799.00</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/238968/1/28904/54806/675bfb59Fe838e691/860fa9b695379f2f.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>100066896420</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro (A3104) 256GB 蓝色钛金属 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100066896420.html</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>8199.00</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/241897/2/29416/53749/675b9857Ffa06ccd3/e0148809ede317c2.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>100067304448</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 15 Pro Max (A3108) 512GB 原色钛金属 支持移动联通电信5G 双卡双待手机【快充套装】</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100067304448.html</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>9488.90</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/200780/10/35055/57366/6500d412F6e866c2e/4cdc1b38cd32d2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>100102229845</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Apple/苹果【24期免息】iPhone 13 (A2634) 256GB 红色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100102229845.html</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>5399.00</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>https://img10.360buyimg.com/n1/jfs/t1/248501/26/10310/28564/66583a09Fc1d7bf2d/039b4af74d9bc2c3.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>100026667892</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Apple/苹果 iPhone 13 (A2634) 512GB 蓝色 支持移动联通电信5G 双卡双待手机</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>https://item.jd.com/100026667892.html</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>5699.00</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Apple产品京东自营旗舰店</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>https://img11.360buyimg.com/n1/jfs/t1/252665/22/83/25601/67614300F3e69b301/da29288df22eade8.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>